<commit_message>
update scenario results v2 xlsx file
</commit_message>
<xml_diff>
--- a/scripts/modeltools/exports/Scenario_Results_v2.xlsx
+++ b/scripts/modeltools/exports/Scenario_Results_v2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\scripts\modeltools\exports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\CDM\scripts\modeltools\exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246AAD52-63BE-4DBE-89CC-015DE55267E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB718105-107C-43D2-99B7-2FF2B3DDDF7D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -576,12 +575,6 @@
     <t>No SE</t>
   </si>
   <si>
-    <t>3A</t>
-  </si>
-  <si>
-    <t>3B</t>
-  </si>
-  <si>
     <t>Life stage: turion viability</t>
   </si>
   <si>
@@ -651,16 +644,22 @@
     <t>% of days where Salt Creek flow is &gt;2 ML/day and average CSL is &gt;+0.8 m AHD</t>
   </si>
   <si>
-    <t>mean concentration (mg/L) between 1 April to 30 September.</t>
-  </si>
-  <si>
-    <t>mean concentration (mg/L) between 1 October to 31 March.</t>
+    <t>Designed</t>
+  </si>
+  <si>
+    <t>No Barrage</t>
+  </si>
+  <si>
+    <t>mean concentration (mg/L) between 1 April - 30 September.</t>
+  </si>
+  <si>
+    <t>mean concentration (mg/L) between 1 October - 31 March.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1191,12 +1190,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3323FCED-6F7F-45C8-A947-57EDCFA88034}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1005" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="L71" sqref="L71:L74"/>
+      <pane ySplit="1005" topLeftCell="A22" activePane="bottomLeft"/>
+      <selection activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="44.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1245,33 +1245,33 @@
         <v>144</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>149</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
@@ -1282,25 +1282,25 @@
     </row>
     <row r="3" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>147</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>149</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>71</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -1311,16 +1311,16 @@
     </row>
     <row r="4" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>19</v>
@@ -1329,7 +1329,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -1340,16 +1340,16 @@
     </row>
     <row r="5" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>19</v>
@@ -1358,7 +1358,7 @@
         <v>71</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -1369,16 +1369,16 @@
     </row>
     <row r="6" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>19</v>
@@ -1387,7 +1387,7 @@
         <v>12</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -1398,16 +1398,16 @@
     </row>
     <row r="7" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>19</v>
@@ -1416,7 +1416,7 @@
         <v>71</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -1427,16 +1427,16 @@
     </row>
     <row r="8" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>21</v>
@@ -1445,7 +1445,7 @@
         <v>12</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -1456,16 +1456,16 @@
     </row>
     <row r="9" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>21</v>
@@ -1474,7 +1474,7 @@
         <v>71</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -1485,16 +1485,16 @@
     </row>
     <row r="10" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>22</v>
@@ -1503,7 +1503,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -1514,16 +1514,16 @@
     </row>
     <row r="11" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>22</v>
@@ -1532,7 +1532,7 @@
         <v>71</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -1543,16 +1543,16 @@
     </row>
     <row r="12" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>22</v>
@@ -1561,7 +1561,7 @@
         <v>12</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
@@ -1572,16 +1572,16 @@
     </row>
     <row r="13" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>22</v>
@@ -1590,7 +1590,7 @@
         <v>71</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -1601,16 +1601,16 @@
     </row>
     <row r="14" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>22</v>
@@ -1619,7 +1619,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -1630,16 +1630,16 @@
     </row>
     <row r="15" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>22</v>
@@ -1648,7 +1648,7 @@
         <v>71</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -1659,25 +1659,25 @@
     </row>
     <row r="16" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>71</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -1688,25 +1688,25 @@
     </row>
     <row r="17" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -1717,25 +1717,25 @@
     </row>
     <row r="18" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C18" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>160</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>162</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -1746,25 +1746,25 @@
     </row>
     <row r="19" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C19" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>160</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>162</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>71</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -1775,25 +1775,25 @@
     </row>
     <row r="20" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -1804,25 +1804,25 @@
     </row>
     <row r="21" spans="1:13" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>71</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -3449,7 +3449,7 @@
         <v>71</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H71">
         <v>82.5137</v>
@@ -3487,7 +3487,7 @@
         <v>71</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -3525,7 +3525,7 @@
         <v>71</v>
       </c>
       <c r="G73" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H73">
         <v>14.2857</v>
@@ -3563,7 +3563,7 @@
         <v>71</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H74">
         <v>0</v>

</xml_diff>